<commit_message>
modified by adding the analysis of percentile, quantile and regression
</commit_message>
<xml_diff>
--- a/iris-2024-01-31.xlsx
+++ b/iris-2024-01-31.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f83c3b872d77321/Desktop/github-projects-data-analysis-ms-excel/Iris-dataset-data-analysis-ms-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="13_ncr:40009_{240B01B6-55D5-470E-B67F-45D0816AEB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FC4137E-9C8B-4F35-8FAB-C36A2B26B28B}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="13_ncr:40009_{240B01B6-55D5-470E-B67F-45D0816AEB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE37506C-3E1D-4BDF-9491-18ED8DD18313}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iris" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="23" r:id="rId5"/>
-    <pivotCache cacheId="18" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="127">
   <si>
     <t>sepal_length</t>
   </si>
@@ -359,12 +359,180 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Regression </t>
+  </si>
+  <si>
+    <t>usually the dependent variable will be in Y axis and independent variable in X axix</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple linear regression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x axis is petal length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y axis is petal area </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentile and Quartile </t>
+  </si>
+  <si>
+    <t>Percentile: It’s a way to measure and express the position of a particular value within a dataset. It tells you what percentage of the data falls below a certain value.</t>
+  </si>
+  <si>
+    <t>Quartiles: Three points that divide a dataset into four equal parts. The first quartile (Q1) is the 25th percentile, the second quartile (Q2) is the median, and the third quartile (Q3) is the 75th percentile.</t>
+  </si>
+  <si>
+    <t>Percentile 0</t>
+  </si>
+  <si>
+    <t>50th percentile</t>
+  </si>
+  <si>
+    <t>75th percentile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100th percentile </t>
+  </si>
+  <si>
+    <t>Quartile 0</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slno </t>
+  </si>
+  <si>
+    <t>minimum value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximum value </t>
+  </si>
+  <si>
+    <t>here n=50 so</t>
+  </si>
+  <si>
+    <t>median= 25.5</t>
+  </si>
+  <si>
+    <t>25th percentile (0.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use the formula of percetile and for k value add the decimal value </t>
+  </si>
+  <si>
+    <t>k=0.25</t>
+  </si>
+  <si>
+    <t>k=0.5</t>
+  </si>
+  <si>
+    <t>k=0.75</t>
+  </si>
+  <si>
+    <t>k=1</t>
+  </si>
+  <si>
+    <t>Q0,P0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1, 25th percentile </t>
+  </si>
+  <si>
+    <t>Q2, 50th percentile</t>
+  </si>
+  <si>
+    <t>Q3 75th percentile</t>
+  </si>
+  <si>
+    <t>Q4, when k in percentile is =1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +726,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF040C28"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF374151"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1006,7 +1181,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1059,20 +1234,22 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1120,6 +1297,51 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -1151,51 +1373,6 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -18835,8 +19012,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5158740" y="21549360"/>
-              <a:ext cx="5973614" cy="2535342"/>
+              <a:off x="6751320" y="21549360"/>
+              <a:ext cx="6628934" cy="2535342"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -19049,8 +19226,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4290060" y="29138880"/>
-              <a:ext cx="5087827" cy="2189583"/>
+              <a:off x="4960620" y="29138880"/>
+              <a:ext cx="6665167" cy="2189583"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -19127,7 +19304,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9906000" y="29039820"/>
+              <a:off x="12153900" y="29039820"/>
               <a:ext cx="3954158" cy="2484120"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -21914,7 +22091,184 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B7851B4-95BB-4A05-852C-F3E8E9E4FE8E}" name="PivotTable15" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+  <location ref="A101:B105" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of petal area" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="10" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="13">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="4"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Iris-20jan2024.xlsx!Table1">
+        <x15:activeTabTopLevelEntity name="[Table1]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{15922D27-C822-4D31-BCEB-CC586503C7B4}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A58:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of petal area" fld="5" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B7851B4-95BB-4A05-852C-F3E8E9E4FE8E}" name="PivotTable15" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A222:C226" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -21965,7 +22319,7 @@
     <dataField name="Min of petal area" fld="5" subtotal="min" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -21977,7 +22331,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -22034,8 +22388,117 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6384F52F-A555-4E63-B141-BCBEF0C7411C}" name="PivotTable28" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A84:E88" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Average of sepal_length" fld="0" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Sum of sepal_width" fld="1" baseField="4" baseItem="0"/>
+    <dataField name="Sum of petal_length" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of petal_width" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="3" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6384F52F-A555-4E63-B141-BCBEF0C7411C}" name="PivotTable28" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A203:C207" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -22095,7 +22558,7 @@
     <dataField name="Min of sepal area" fld="6" subtotal="min" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="4">
+    <format dxfId="8">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -22107,7 +22570,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -22119,7 +22582,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -22326,378 +22789,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A136:B140" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of petal_width" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable3" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
-  <location ref="A101:B105" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of petal area" fld="1" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="10" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotHierarchies count="13">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="4"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Iris-20jan2024.xlsx!Table1">
-        <x15:activeTabTopLevelEntity name="[Table1]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A84:E88" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="4">
-    <dataField name="Average of sepal_length" fld="0" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Sum of sepal_width" fld="1" baseField="4" baseItem="0"/>
-    <dataField name="Sum of petal_length" fld="2" baseField="0" baseItem="0"/>
-    <dataField name="Sum of petal_width" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="3" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="11" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{15922D27-C822-4D31-BCEB-CC586503C7B4}" name="PivotTable12" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A58:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Max of petal area" fld="5" subtotal="max" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="5">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2158D523-B4D4-4FB3-A2A0-1F77DA3C6FF7}" name="PivotTable11" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2158D523-B4D4-4FB3-A2A0-1F77DA3C6FF7}" name="PivotTable11" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A22:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -22797,6 +22890,90 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A136:B140" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of petal_width" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G151" totalsRowShown="0">
   <autoFilter ref="A1:G151" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -22814,7 +22991,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D21192DB-576A-4F78-A140-9DDEFAA8FBA0}" name="Table35" displayName="Table35" ref="F39:F53" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D21192DB-576A-4F78-A140-9DDEFAA8FBA0}" name="Table35" displayName="Table35" ref="F39:F53" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="F39:F53" xr:uid="{D21192DB-576A-4F78-A140-9DDEFAA8FBA0}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A9E6045E-5DD9-4B48-A2CC-314D9D2EA812}" name="Petal Area">
@@ -23124,8 +23301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26623,10 +26800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C81BAF2-CCCF-462A-91D3-6EFD84BEE3EC}">
-  <dimension ref="A1:O246"/>
+  <dimension ref="A1:O342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="I348" sqref="I348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26645,7 +26822,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="33" t="s">
         <v>56</v>
       </c>
     </row>
@@ -26760,7 +26937,7 @@
         <f t="shared" ref="F41:F53" si="0">C41*D41</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H41" s="38"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
@@ -27031,10 +27208,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="34" t="s">
+      <c r="A59" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="33">
+      <c r="B59" s="30">
         <v>15.87</v>
       </c>
     </row>
@@ -27042,7 +27219,7 @@
       <c r="A60" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="32">
+      <c r="B60">
         <v>8.64</v>
       </c>
     </row>
@@ -27050,7 +27227,7 @@
       <c r="A61" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="32">
+      <c r="B61">
         <v>0.96</v>
       </c>
     </row>
@@ -27058,7 +27235,7 @@
       <c r="A62" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B62" s="32">
+      <c r="B62">
         <v>15.87</v>
       </c>
     </row>
@@ -27507,7 +27684,7 @@
       <c r="E156" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F156" s="39" t="s">
+      <c r="F156" s="35" t="s">
         <v>70</v>
       </c>
     </row>
@@ -27789,10 +27966,10 @@
       <c r="A204" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B204" s="36">
+      <c r="B204">
         <v>7.5</v>
       </c>
-      <c r="C204" s="32">
+      <c r="C204">
         <v>12.25</v>
       </c>
     </row>
@@ -27800,10 +27977,10 @@
       <c r="A205" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B205" s="33">
+      <c r="B205" s="30">
         <v>0.11000000000000001</v>
       </c>
-      <c r="C205" s="32">
+      <c r="C205">
         <v>10.35</v>
       </c>
     </row>
@@ -27811,10 +27988,10 @@
       <c r="A206" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B206" s="32">
+      <c r="B206">
         <v>3.3</v>
       </c>
-      <c r="C206" s="33">
+      <c r="C206" s="30">
         <v>10</v>
       </c>
     </row>
@@ -27822,10 +27999,10 @@
       <c r="A207" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B207" s="32">
+      <c r="B207">
         <v>0.11000000000000001</v>
       </c>
-      <c r="C207" s="32">
+      <c r="C207">
         <v>10</v>
       </c>
     </row>
@@ -27881,10 +28058,10 @@
       <c r="A223" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B223" s="32">
+      <c r="B223">
         <v>0.96</v>
       </c>
-      <c r="C223" s="32">
+      <c r="C223">
         <v>0.11000000000000001</v>
       </c>
     </row>
@@ -27892,10 +28069,10 @@
       <c r="A224" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B224" s="32">
+      <c r="B224">
         <v>8.64</v>
       </c>
-      <c r="C224" s="32">
+      <c r="C224">
         <v>3.3</v>
       </c>
     </row>
@@ -27903,10 +28080,10 @@
       <c r="A225" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B225" s="37">
+      <c r="B225" s="34">
         <v>15.87</v>
       </c>
-      <c r="C225" s="32">
+      <c r="C225">
         <v>7.5</v>
       </c>
     </row>
@@ -27914,10 +28091,10 @@
       <c r="A226" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B226" s="32">
+      <c r="B226">
         <v>15.87</v>
       </c>
-      <c r="C226" s="32">
+      <c r="C226">
         <v>0.11000000000000001</v>
       </c>
     </row>
@@ -27951,7 +28128,942 @@
         <v>setosa</v>
       </c>
     </row>
+    <row r="263" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A263" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B263" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>73</v>
+      </c>
+      <c r="B267" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D267" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D268" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A269" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B269" s="17"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>75</v>
+      </c>
+      <c r="B270">
+        <v>0.95847223975235052</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>76</v>
+      </c>
+      <c r="B271">
+        <v>0.91866903437588732</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>77</v>
+      </c>
+      <c r="B272">
+        <v>0.91811950082437299</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>23</v>
+      </c>
+      <c r="B273">
+        <v>1.3487568350773402</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A274" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B274" s="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A277" s="16"/>
+      <c r="B277" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C277" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D277" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E277" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F277" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>80</v>
+      </c>
+      <c r="B278">
+        <v>1</v>
+      </c>
+      <c r="C278">
+        <v>3041.1103673084926</v>
+      </c>
+      <c r="D278">
+        <v>3041.1103673084926</v>
+      </c>
+      <c r="E278">
+        <v>1671.7251054907138</v>
+      </c>
+      <c r="F278">
+        <v>1.5601948101150016E-82</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>81</v>
+      </c>
+      <c r="B279">
+        <v>148</v>
+      </c>
+      <c r="C279">
+        <v>269.23346002484084</v>
+      </c>
+      <c r="D279">
+        <v>1.8191450001678435</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A280" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B280" s="15">
+        <v>149</v>
+      </c>
+      <c r="C280" s="15">
+        <v>3310.3438273333336</v>
+      </c>
+      <c r="D280" s="15"/>
+      <c r="E280" s="15"/>
+      <c r="F280" s="15"/>
+    </row>
+    <row r="281" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A282" s="16"/>
+      <c r="B282" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C282" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D282" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E282" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F282" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G282" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H282" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I282" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>83</v>
+      </c>
+      <c r="B283">
+        <v>-3.830846268645562</v>
+      </c>
+      <c r="C283">
+        <v>0.25986932754340464</v>
+      </c>
+      <c r="D283">
+        <v>-14.741432953474339</v>
+      </c>
+      <c r="E283">
+        <v>7.7507072120495959E-31</v>
+      </c>
+      <c r="F283">
+        <v>-4.344379892204361</v>
+      </c>
+      <c r="G283">
+        <v>-3.3173126450867625</v>
+      </c>
+      <c r="H283">
+        <v>-4.344379892204361</v>
+      </c>
+      <c r="I283">
+        <v>-3.3173126450867625</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A284" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B284" s="15">
+        <v>2.5604770136517088</v>
+      </c>
+      <c r="C284" s="15">
+        <v>6.2623660428022393E-2</v>
+      </c>
+      <c r="D284" s="15">
+        <v>40.886735079860721</v>
+      </c>
+      <c r="E284" s="15">
+        <v>1.5601948101150458E-82</v>
+      </c>
+      <c r="F284" s="15">
+        <v>2.4367249896474648</v>
+      </c>
+      <c r="G284" s="15">
+        <v>2.6842290376559528</v>
+      </c>
+      <c r="H284" s="15">
+        <v>2.4367249896474648</v>
+      </c>
+      <c r="I284" s="15">
+        <v>2.6842290376559528</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A287" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A289" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A290" s="37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A292" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B292" s="21">
+        <f>PERCENTILE(G293:G342,0)</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="C292" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D292" s="21"/>
+      <c r="F292" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G292" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H292" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A293" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B293" s="21">
+        <f>PERCENTILE(G293:G342,0.25)</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C293" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D293" s="21"/>
+      <c r="F293" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G293" s="38">
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="H293">
+        <v>1</v>
+      </c>
+      <c r="I293" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A294" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B294" s="21">
+        <f>PERCENTILE(G293:G342,0.5)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C294" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D294" s="21"/>
+      <c r="F294" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G294" s="39">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="H294">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A295" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B295" s="21">
+        <f>PERCENTILE(G293:G342,0.75)</f>
+        <v>0.42</v>
+      </c>
+      <c r="C295" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D295" s="21"/>
+      <c r="F295" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G295" s="38">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H295">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A296" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B296" s="21">
+        <f>PERCENTILE(G293:G342,1)</f>
+        <v>0.96</v>
+      </c>
+      <c r="C296" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D296" s="21"/>
+      <c r="F296" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G296" s="39">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H296">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F297" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G297" s="39">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H297">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A298" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B298" s="21">
+        <f>QUARTILE(G293:G342,0)</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="C298" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D298" s="21">
+        <f>MIN(G293:G342)</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="F298" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G298" s="38">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H298">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A299" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B299" s="21">
+        <f>QUARTILE(G293:G342,1)</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C299" s="21"/>
+      <c r="D299" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F299" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G299" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="H299">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A300" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B300" s="21">
+        <f>QUARTILE(G293:G342,2)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C300" s="21"/>
+      <c r="D300" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F300" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G300" s="39">
+        <v>0.24</v>
+      </c>
+      <c r="H300">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A301" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B301" s="21">
+        <f>QUARTILE(G293:G342,3)</f>
+        <v>0.42</v>
+      </c>
+      <c r="C301" s="21"/>
+      <c r="D301" s="21"/>
+      <c r="F301" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G301" s="38">
+        <v>0.24</v>
+      </c>
+      <c r="H301">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A302" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B302" s="21">
+        <f>QUARTILE(G293:G342,4)</f>
+        <v>0.96</v>
+      </c>
+      <c r="C302" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D302" s="21">
+        <f>MAX(G293:G342)</f>
+        <v>0.96</v>
+      </c>
+      <c r="F302" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G302" s="39">
+        <v>0.26</v>
+      </c>
+      <c r="H302">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F303" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G303" s="39">
+        <v>0.26</v>
+      </c>
+      <c r="H303">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F304" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G304" s="39">
+        <v>0.26</v>
+      </c>
+      <c r="H304">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="305" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F305" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G305" s="39">
+        <v>0.26</v>
+      </c>
+      <c r="H305">
+        <v>13</v>
+      </c>
+      <c r="I305" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="306" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F306" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G306" s="39">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H306">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="307" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F307" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G307" s="38">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H307">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="308" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F308" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G308" s="39">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H308">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="309" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F309" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G309" s="39">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H309">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="310" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F310" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G310" s="39">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H310">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="311" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F311" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G311" s="38">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H311">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="312" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F312" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G312" s="38">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H312">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="313" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F313" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G313" s="38">
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="H313">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="314" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F314" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G314" s="38">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H314">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="315" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F315" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G315" s="38">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H315">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="316" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F316" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G316" s="39">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H316">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="317" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F317" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G317" s="38">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H317">
+        <v>25</v>
+      </c>
+      <c r="I317" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="318" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F318" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G318" s="38">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H318">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="319" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F319" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G319" s="39">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H319">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="320" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F320" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G320" s="38">
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="H320">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="321" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F321" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G321" s="38">
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="H321">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="322" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F322" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G322" s="38">
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="H322">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="323" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F323" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G323" s="39">
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="H323">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="324" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F324" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G324" s="39">
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="H324">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="325" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F325" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G325" s="39">
+        <v>0.34</v>
+      </c>
+      <c r="H325">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="326" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F326" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G326" s="39">
+        <v>0.38</v>
+      </c>
+      <c r="H326">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="327" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F327" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G327" s="39">
+        <v>0.39</v>
+      </c>
+      <c r="H327">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="328" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F328" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G328" s="38">
+        <v>0.39</v>
+      </c>
+      <c r="H328">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="329" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F329" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G329" s="39">
+        <v>0.42</v>
+      </c>
+      <c r="H329">
+        <v>37</v>
+      </c>
+      <c r="I329" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="330" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F330" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G330" s="38">
+        <v>0.42</v>
+      </c>
+      <c r="H330">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="331" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F331" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G331" s="38">
+        <v>0.42</v>
+      </c>
+      <c r="H331">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="332" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F332" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G332" s="38">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="H332">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="333" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F333" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G333" s="39">
+        <v>0.51</v>
+      </c>
+      <c r="H333">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="334" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F334" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G334" s="39">
+        <v>0.52</v>
+      </c>
+      <c r="H334">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="335" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F335" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G335" s="38">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H335">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="336" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F336" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G336" s="38">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H336">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="337" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F337" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G337" s="38">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H337">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="338" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F338" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G338" s="39">
+        <v>0.64000000000000012</v>
+      </c>
+      <c r="H338">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="339" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F339" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G339" s="38">
+        <v>0.68</v>
+      </c>
+      <c r="H339">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="340" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F340" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G340" s="39">
+        <v>0.76</v>
+      </c>
+      <c r="H340">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="341" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F341" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G341" s="38">
+        <v>0.85</v>
+      </c>
+      <c r="H341">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="342" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F342" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G342" s="38">
+        <v>0.96</v>
+      </c>
+      <c r="H342">
+        <v>50</v>
+      </c>
+      <c r="I342" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F293:H342">
+    <sortCondition ref="G292:G342"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId8"/>
   <tableParts count="1">

</xml_diff>